<commit_message>
Finished the poster; Got the DDTW to work... blah, it's slow.
</commit_message>
<xml_diff>
--- a/docs/Plots & Analysis/CPU Analysis.xlsx
+++ b/docs/Plots & Analysis/CPU Analysis.xlsx
@@ -16,31 +16,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>No optimisation</t>
+    <t>Width in %</t>
   </si>
   <si>
-    <t>Sakoe-Chiba</t>
+    <t>Optimization</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>Procentage</t>
+    <t>Calculations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,7 +59,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,15 +67,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -370,293 +387,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E7" sqref="B1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D2">
+        <f t="shared" ref="D2:D7" si="0">B2*(2*C2-1) - C2*C2 - 1</f>
+        <v>295</v>
+      </c>
+      <c r="E2" s="1">
+        <f xml:space="preserve"> (1 - D2/(B2*B2))</f>
+        <v>0.97050000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>683</v>
+      </c>
+      <c r="E3" s="1">
+        <f xml:space="preserve"> (1 - D3/(B3*B3))</f>
+        <v>0.93169999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>100</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <f>A2*A2</f>
-        <v>10000</v>
-      </c>
-      <c r="E2">
-        <f>A2*(2*B2-1) - B2*B2 - 1</f>
-        <v>295</v>
-      </c>
-      <c r="F2" s="1">
-        <f xml:space="preserve"> (1 - E2/D2)</f>
-        <v>0.97050000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1063</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E7" si="1" xml:space="preserve"> (1 - D4/(B4*B4))</f>
+        <v>0.89369999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>100</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <f>A3*A3</f>
-        <v>10000</v>
-      </c>
-      <c r="E3">
-        <f>A3*(2*B3-1) - B3*B3 - 1</f>
-        <v>683</v>
-      </c>
-      <c r="F3" s="1">
-        <f xml:space="preserve"> (1 - E3/D3)</f>
-        <v>0.93169999999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>100</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D7" si="0">A4*A4</f>
-        <v>10000</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E7" si="1">A4*(2*B4-1) - B4*B4 - 1</f>
-        <v>1063</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" ref="F4:F7" si="2" xml:space="preserve"> (1 - E4/D4)</f>
-        <v>0.89369999999999994</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>100</v>
-      </c>
-      <c r="B5">
+      <c r="C5">
         <v>8</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>10000</v>
-      </c>
-      <c r="E5">
+        <v>1435</v>
+      </c>
+      <c r="E5" s="1">
         <f t="shared" si="1"/>
-        <v>1435</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="2"/>
         <v>0.85650000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>100</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>10</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>10000</v>
-      </c>
-      <c r="E6">
+        <v>1799</v>
+      </c>
+      <c r="E6" s="1">
         <f t="shared" si="1"/>
-        <v>1799</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="2"/>
         <v>0.82010000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>100</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>12</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>10000</v>
-      </c>
-      <c r="E7">
+        <v>2155</v>
+      </c>
+      <c r="E7" s="1">
         <f t="shared" si="1"/>
-        <v>2155</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="2"/>
         <v>0.78449999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1024</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="D10">
-        <f>A10*A10</f>
-        <v>1048576</v>
-      </c>
-      <c r="E10">
-        <f>A10*(2*B10-1) - B10*B10 - 1</f>
-        <v>3067</v>
-      </c>
-      <c r="F10" s="1">
-        <f xml:space="preserve"> (1 - E10/D10)</f>
-        <v>0.99707508087158203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="e">
+        <f xml:space="preserve"> (1 -#REF! /#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1024</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
-      <c r="D11">
-        <f>A11*A11</f>
-        <v>1048576</v>
-      </c>
-      <c r="E11">
-        <f>A11*(2*B11-1) - B11*B11 - 1</f>
-        <v>7151</v>
-      </c>
-      <c r="F11" s="1">
-        <f xml:space="preserve"> (1 - E11/D11)</f>
-        <v>0.99318027496337891</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="e">
+        <f xml:space="preserve"> (1 -#REF! /#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1024</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
-      <c r="D12">
-        <f t="shared" ref="D12:D15" si="3">A12*A12</f>
-        <v>1048576</v>
-      </c>
-      <c r="E12">
-        <f t="shared" ref="E12:E15" si="4">A12*(2*B12-1) - B12*B12 - 1</f>
-        <v>11227</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" ref="F12:F15" si="5" xml:space="preserve"> (1 - E12/D12)</f>
-        <v>0.98929309844970703</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="e">
+        <f xml:space="preserve"> (1 -#REF! /#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1024</v>
       </c>
       <c r="B13">
         <v>8</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="3"/>
-        <v>1048576</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="4"/>
-        <v>15295</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="5"/>
-        <v>0.98541355133056641</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="e">
+        <f xml:space="preserve"> (1 -#REF! /#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1024</v>
       </c>
       <c r="B14">
         <v>10</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="3"/>
-        <v>1048576</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="4"/>
-        <v>19355</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="5"/>
-        <v>0.98154163360595703</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="e">
+        <f xml:space="preserve"> (1 -#REF! /#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1024</v>
       </c>
       <c r="B15">
         <v>12</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="3"/>
-        <v>1048576</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="4"/>
-        <v>23407</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="5"/>
-        <v>0.97767734527587891</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="1"/>
+      <c r="D15" s="1" t="e">
+        <f xml:space="preserve"> (1 -#REF! /#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>